<commit_message>
Deploying to gh-pages from @ torstees/ncpi-fhir-ig-2@537984b1c0b3db4c39b833973081dfc1c90611e0 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-collection-type.xlsx
+++ b/CodeSystem-collection-type.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://nih-ncpi.github.ioo/ncpi-fhir-ig-2/CodeSystem/collection-type</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig-2/CodeSystem/collection-type</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-03T22:56:43+00:00</t>
+    <t>2024-03-11T22:11:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>